<commit_message>
arreglo en el catalogo
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\MODIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770A5192-0B8B-4633-8746-F4FF09BA39C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CDB0F4-1368-44F1-9F2F-19BF60D0C44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="599" activeTab="1" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" activeTab="1" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,10 +524,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC3386-F6B0-4296-A730-E04C7B4A8BD3}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +941,7 @@
       <c r="L2" t="s">
         <v>89</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="5" t="s">
         <v>142</v>
       </c>
     </row>
@@ -983,220 +982,220 @@
       <c r="L3" s="4">
         <v>183.76</v>
       </c>
-      <c r="M3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="M3" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>4.5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>5</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>5</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="6">
         <v>5</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <v>5</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="6">
         <v>5</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="6">
         <v>5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>5</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="M4" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="6">
         <v>1.95</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>2.1800000000000002</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="6">
         <f>+E16*E17</f>
         <v>2.1777440000000001</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <f t="shared" ref="F5:L5" si="0">+F16*F17</f>
         <v>2.1526999999999998</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="6">
         <f t="shared" si="0"/>
         <v>2.1736</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="6">
         <f t="shared" si="0"/>
         <v>2.8210000000000002</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="6">
         <f t="shared" si="0"/>
         <v>2.5763999999999996</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="6">
         <f t="shared" si="0"/>
         <v>2.1840000000000002</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="6">
         <f t="shared" si="0"/>
         <v>22.302399999999999</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="6">
         <f t="shared" si="0"/>
         <v>22.302399999999999</v>
       </c>
-      <c r="M5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="M5" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>370</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>450</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>445</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>465</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>445</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>590</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>540</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>450</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>455</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>450</v>
       </c>
-      <c r="M6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="M6" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>25</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>25</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>25</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>25</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>25</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="6">
         <v>25</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="6">
         <v>25</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="6">
         <v>25</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="6">
         <v>25</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>25</v>
       </c>
-      <c r="M7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="M7" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>0.65</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>0.65</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>0.65</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>0.65</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <v>0.65</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="6">
         <v>0.65</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
         <v>0.65</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="6">
         <v>0.65</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="6">
         <v>0.65</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>0.65</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="5" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1216,34 +1215,34 @@
       <c r="E9" s="4">
         <v>49.07</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>51.92</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>50.1</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>41.2</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>49.4</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>50</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>49.85</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <v>49.7</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="M9" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1261,34 +1260,34 @@
       <c r="E10" s="4">
         <v>11.46</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>11.59</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>11.4</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>18.21</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>13.81</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>11.44</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>11.41</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <v>11.36</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
+      <c r="M10" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1306,34 +1305,34 @@
       <c r="E11" s="4">
         <v>41.17</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>43.18</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>41.2</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>34.32</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>41.2</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>41.4</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>41.82</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>41.52</v>
       </c>
-      <c r="M11" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="M11" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1351,34 +1350,34 @@
       <c r="E12" s="4">
         <v>10.81</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>10.77</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>10.81</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>17.2</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>13.11</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>10.87</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>10.88</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>10.84</v>
       </c>
-      <c r="M12" t="s">
-        <v>142</v>
-      </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="M12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1396,34 +1395,34 @@
       <c r="E13" s="4">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>-0.25</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>-0.3</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>-0.27</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <v>-0.27</v>
       </c>
-      <c r="M13" t="s">
-        <v>142</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
+      <c r="M13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1441,34 +1440,34 @@
       <c r="E14" s="4">
         <v>0.05</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>0.05</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>0.05</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>0.04</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <v>0.05</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>0.05</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="M14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1486,34 +1485,34 @@
       <c r="E15" s="4">
         <v>-0.35</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>-0.36</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>-0.36</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>-0.34</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>-0.36</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <v>-0.35</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>-0.35</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="6">
         <v>-0.35</v>
       </c>
-      <c r="M15" t="s">
-        <v>142</v>
-      </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
+      <c r="M15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1531,34 +1530,34 @@
       <c r="E16" s="4">
         <v>2.0960000000000001</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>2.09</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>2.09</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>2.17</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>2.2799999999999998</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>2.1</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>2.12</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>2.12</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+      <c r="M16" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1576,28 +1575,28 @@
       <c r="E17" s="4">
         <v>1.0389999999999999</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>1.03</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>1.04</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>1.3</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>1.1299999999999999</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <v>1.04</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>10.52</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="6">
         <v>10.52</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="M17" s="5" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1610,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8590178-7E48-4D91-905D-79485D6F38C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,446 +1740,446 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <v>2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="5">
         <v>2</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="5">
         <v>2</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="L4" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>4.8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>2.56</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>2.4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>3.2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <v>4.8</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>3.3744000000000001</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>3.84</v>
       </c>
-      <c r="L5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="L5" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.24</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>0.51200000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>0.12</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>0.32</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="5">
         <v>0.48</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>0.255</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <f>+I5*0.1</f>
         <v>0.33744000000000002</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>0.22</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <f>+K5*0.1</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="L6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="L6" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>2.4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>1.28</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <f t="shared" ref="E7:K7" si="0">+E5*E15</f>
         <v>2.4</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>3.7919999999999998</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <f t="shared" si="0"/>
         <v>3.3744000000000001</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="5">
         <f t="shared" si="0"/>
         <v>1.254</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
-      <c r="L7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="L7" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>2.4</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>1.28</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <f>+E5*E15</f>
         <v>2.4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <f t="shared" ref="F8:K8" si="1">+F5*F15</f>
         <v>3.2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>3.7919999999999998</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>2.5499999999999998</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <f t="shared" si="1"/>
         <v>3.3744000000000001</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="5">
         <f t="shared" si="1"/>
         <v>1.254</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <f t="shared" si="1"/>
         <v>3.84</v>
       </c>
-      <c r="L8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="L8" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>0.98</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>0.98</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>0.98</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>0.98</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="5">
         <v>0.98</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="5">
         <v>0.98</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="5">
         <v>0.98</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="5">
         <v>0.98</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="5">
         <v>0.98</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="L9" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>13</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>13</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>15</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>10</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>10</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>10</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>15</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>15</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>10</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="L10" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>48</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>48</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>48</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>48</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>48</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>48</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>48</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="5">
         <v>48</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="5">
         <v>48</v>
       </c>
-      <c r="L11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="L11" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>4500</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>6000</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>6000</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="5">
         <v>6000</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
         <v>6000</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>6000</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <v>6000</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <v>6000</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="5">
         <v>6000</v>
       </c>
-      <c r="L12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="L12" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f t="shared" ref="C13:K13" si="2">((0.2*C5)/C12)/(C5-C6)</f>
         <v>4.6783625730994155E-5</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f t="shared" si="2"/>
         <v>4.1666666666666665E-5</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f t="shared" si="2"/>
         <v>3.5087719298245611E-5</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <f t="shared" si="2"/>
         <v>3.7037037037037043E-5</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f t="shared" si="2"/>
         <v>3.703703703703703E-5</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <f t="shared" si="2"/>
         <v>3.7037037037037043E-5</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <f t="shared" si="2"/>
         <v>3.7037037037037037E-5</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
+        <f>((0.2*J5)/J12)/(J5-J6)</f>
+        <v>3.7037037037037037E-5</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="2"/>
         <v>3.7037037037037037E-5</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="2"/>
-        <v>3.7037037037037037E-5</v>
-      </c>
-      <c r="L13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="L13" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="5">
         <v>1.075E-4</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="5" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Determinación del pais y ciudad por medio de la ubicación
</commit_message>
<xml_diff>
--- a/Catalogo.xlsx
+++ b/Catalogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\MODIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CDB0F4-1368-44F1-9F2F-19BF60D0C44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7E7F03-4F73-4234-9663-B660397EBE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" activeTab="1" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="599" activeTab="5" xr2:uid="{27070F80-89CF-4E15-8F14-835BDE193743}"/>
   </bookViews>
   <sheets>
     <sheet name="PVModules" sheetId="25" r:id="rId1"/>
@@ -490,18 +490,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -516,13 +510,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -941,7 +934,7 @@
       <c r="L2" t="s">
         <v>89</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -952,250 +945,250 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>187.89</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>206.5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>189.44</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>196.38</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>1998.69</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>275.02</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>253.24</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>205.85</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>194.55</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>183.76</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="M3" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>4.5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>5</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>5</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>5</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>5</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>5</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="M4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1.95</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>2.1800000000000002</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f>+E16*E17</f>
         <v>2.1777440000000001</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f t="shared" ref="F5:L5" si="0">+F16*F17</f>
         <v>2.1526999999999998</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>2.1736</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
         <v>2.8210000000000002</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f t="shared" si="0"/>
         <v>2.5763999999999996</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f t="shared" si="0"/>
         <v>2.1840000000000002</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <f t="shared" si="0"/>
         <v>22.302399999999999</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <f t="shared" si="0"/>
         <v>22.302399999999999</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="M5" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>370</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>450</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>445</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>465</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>445</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>590</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>540</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>450</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>455</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>450</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="M6" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>25</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>25</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>25</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>25</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>25</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>25</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>25</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>25</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>25</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>25</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="M7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.65</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.65</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.65</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>0.65</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.65</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>0.65</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>0.65</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>0.65</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>0.65</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>0.65</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1206,43 +1199,43 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>48.3</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>49.98</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>49.07</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>51.92</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>50.1</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>41.2</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>49.4</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>50</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>49.85</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>49.7</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="M9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1251,43 +1244,43 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>9.85</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>11.54</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>11.46</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>11.59</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>11.4</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>18.21</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>13.81</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>11.44</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>11.41</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>11.36</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="M10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1296,43 +1289,43 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>39.299999999999997</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>41.4</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>41.17</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>43.18</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>41.2</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>34.32</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>41.2</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>41.4</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>41.82</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>41.52</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="M11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1341,43 +1334,43 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>9.41</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>10.87</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>10.81</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>10.77</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>10.81</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>17.2</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>13.11</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>10.87</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>10.88</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="5">
         <v>10.84</v>
       </c>
-      <c r="M12" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="M12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1386,43 +1379,43 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>-0.25</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>-0.3</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>-0.27</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>-0.27</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="M13" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1431,43 +1424,43 @@
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>0.05</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>0.05</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0.05</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>0.05</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>0.05</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>0.04</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>0.05</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>0.05</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="M14" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1476,43 +1469,43 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>-0.4</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>-0.36</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>-0.35</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>-0.36</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>-0.36</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>-0.34</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>-0.36</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>-0.35</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>-0.35</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>-0.35</v>
       </c>
-      <c r="M15" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
+      <c r="M15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1521,43 +1514,43 @@
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>1.95</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>2.0950000000000002</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>2.0960000000000001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>2.09</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>2.09</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>2.17</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <v>2.2799999999999998</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>2.1</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>2.12</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="5">
         <v>2.12</v>
       </c>
-      <c r="M16" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+      <c r="M16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1566,37 +1559,37 @@
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>1.0389999999999999</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>1.0389999999999999</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>1.03</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>1.04</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>1.3</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>1.1299999999999999</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>1.04</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>10.52</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <v>10.52</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1609,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8590178-7E48-4D91-905D-79485D6F38C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -1740,446 +1733,446 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>2</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>2</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>2</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>2</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="L4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>4.8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2.56</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>2.4</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>3.2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>4.8</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>3.3744000000000001</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>3.84</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="L5" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.24</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.51200000000000001</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.12</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.32</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.48</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0.255</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f>+I5*0.1</f>
         <v>0.33744000000000002</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>0.22</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <f>+K5*0.1</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="L6" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>2.4</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>1.28</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" ref="E7:K7" si="0">+E5*E15</f>
         <v>2.4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>3.7919999999999998</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>2.5499999999999998</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>3.3744000000000001</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>1.254</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
         <v>3.84</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="L7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2.4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>1.28</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f>+E5*E15</f>
         <v>2.4</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" ref="F8:K8" si="1">+F5*F15</f>
         <v>3.2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
         <v>3.7919999999999998</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <f t="shared" si="1"/>
         <v>2.5499999999999998</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f t="shared" si="1"/>
         <v>3.3744000000000001</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <f t="shared" si="1"/>
         <v>1.254</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <f t="shared" si="1"/>
         <v>3.84</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="L8" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.98</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0.98</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0.98</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.98</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>0.98</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>0.98</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>0.98</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>0.98</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>0.98</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="L9" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>13</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>13</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>15</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>10</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>10</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>10</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>15</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>15</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <v>10</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="L10" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>48</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>48</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>48</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>48</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>48</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>48</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>48</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>48</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>48</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="L11" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>4500</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>6000</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>6000</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>6000</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>6000</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>6000</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>6000</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>6000</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>6000</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="L12" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f t="shared" ref="C13:K13" si="2">((0.2*C5)/C12)/(C5-C6)</f>
         <v>4.6783625730994155E-5</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f t="shared" si="2"/>
         <v>4.1666666666666665E-5</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="2"/>
         <v>3.5087719298245611E-5</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="2"/>
         <v>3.7037037037037043E-5</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="2"/>
         <v>3.703703703703703E-5</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <f t="shared" si="2"/>
         <v>3.7037037037037043E-5</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <f t="shared" si="2"/>
         <v>3.7037037037037037E-5</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <f>((0.2*J5)/J12)/(J5-J6)</f>
         <v>3.7037037037037037E-5</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <f t="shared" si="2"/>
         <v>3.7037037037037037E-5</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="L13" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="4">
         <v>1.075E-4</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2324,7 +2317,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E1" sqref="E1:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2342,7 @@
       <c r="D1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2366,7 +2359,7 @@
       <c r="D2">
         <v>2126</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2383,7 +2376,7 @@
       <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2400,7 +2393,7 @@
       <c r="D4">
         <v>6.65</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2417,7 +2410,7 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2434,7 +2427,7 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2451,7 +2444,7 @@
       <c r="D7">
         <v>600</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2468,7 +2461,7 @@
       <c r="D8">
         <v>120</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2485,7 +2478,7 @@
       <c r="D9">
         <v>360</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2502,7 +2495,7 @@
       <c r="D10">
         <v>15</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2519,7 +2512,7 @@
       <c r="D11">
         <v>0.94</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2536,7 +2529,7 @@
       <c r="D12">
         <v>0.95</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2553,7 +2546,7 @@
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2570,7 +2563,7 @@
       <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2587,7 +2580,7 @@
       <c r="D15">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2604,7 +2597,7 @@
       <c r="D16">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2621,7 +2614,7 @@
       <c r="D17">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2638,7 +2631,7 @@
       <c r="D18">
         <v>140</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2655,7 +2648,7 @@
       <c r="D19">
         <v>140</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2672,7 +2665,7 @@
       <c r="D20">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2686,7 +2679,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,7 +2704,7 @@
       <c r="E1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2731,7 +2724,7 @@
       <c r="E2" t="s">
         <v>123</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2751,7 +2744,7 @@
       <c r="E3">
         <v>1100</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2771,7 +2764,7 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2791,7 +2784,7 @@
       <c r="E5">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2811,7 +2804,7 @@
       <c r="E6">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2831,7 +2824,7 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2851,7 +2844,7 @@
       <c r="E8">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2871,7 +2864,7 @@
       <c r="E9">
         <v>20</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2884,7 +2877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CC0D24-3C64-426B-B862-F2C03B105542}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>